<commit_message>
Added New testscripts - modified old test scripts
All the modified and added test scripts were successfully tested in local . Old test scripts from prior sprints were modified as per the latest session compatibility
</commit_message>
<xml_diff>
--- a/cypress/cypressTestProgressTracker.xlsx
+++ b/cypress/cypressTestProgressTracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26322"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bhuvana\MS-Course\MIS-Spring2023\ISQA8950\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kisho\Documents\Projects\uno-cpi\cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="166" documentId="8_{05AFC60E-9732-4AAD-88BE-F454733218E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{471C66A5-A249-42F9-85D4-F26BBBDCE68E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BEC1B27-9041-4CDD-A8B6-3D3AC1DE5A2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories (+issues stories)" sheetId="10" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Open Issues'!$A$1:$O$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'User Stories (+issues stories)'!$A$1:$BR$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'User Stories (+issues stories)'!$A$1:$BR$63</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="328">
   <si>
     <t>SNO</t>
   </si>
@@ -2802,7 +2802,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3612,32 +3612,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3919,13 +3919,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF50C64C-9D5B-44C0-8C71-AEDF26F82C35}">
-  <dimension ref="A1:BR89"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:BR87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="J63" sqref="J63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.7109375" style="4"/>
     <col min="2" max="2" width="12.7109375" style="23" customWidth="1"/>
@@ -3940,7 +3941,7 @@
     <col min="13" max="16384" width="8.7109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:70" ht="45.75">
+    <row r="1" spans="1:70" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3981,7 +3982,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:70" ht="30.75">
+    <row r="2" spans="1:70" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -4019,7 +4020,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:70" ht="30.75">
+    <row r="3" spans="1:70" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -4057,7 +4058,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:70" ht="28.9">
+    <row r="4" spans="1:70" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -4089,7 +4090,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:70" s="47" customFormat="1" ht="28.9">
+    <row r="5" spans="1:70" s="47" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="47">
         <v>4</v>
       </c>
@@ -4121,7 +4122,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:70" s="51" customFormat="1" ht="28.9">
+    <row r="6" spans="1:70" s="51" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="51">
         <v>5</v>
       </c>
@@ -4155,7 +4156,7 @@
       <c r="K6" s="47"/>
       <c r="L6" s="47"/>
     </row>
-    <row r="7" spans="1:70" s="51" customFormat="1" ht="28.9">
+    <row r="7" spans="1:70" s="51" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="51">
         <v>6</v>
       </c>
@@ -4189,7 +4190,7 @@
       <c r="K7" s="47"/>
       <c r="L7" s="47"/>
     </row>
-    <row r="8" spans="1:70" s="8" customFormat="1" ht="28.9">
+    <row r="8" spans="1:70" s="8" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -4221,7 +4222,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:70" ht="28.9">
+    <row r="9" spans="1:70" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -4253,7 +4254,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:70" s="8" customFormat="1" ht="28.9">
+    <row r="10" spans="1:70" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>9</v>
       </c>
@@ -4285,7 +4286,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:70" s="21" customFormat="1" ht="28.9">
+    <row r="11" spans="1:70" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="37">
         <v>10</v>
       </c>
@@ -4360,7 +4361,7 @@
       <c r="AZ11" s="37"/>
       <c r="BA11" s="37"/>
     </row>
-    <row r="12" spans="1:70" s="47" customFormat="1" ht="28.9">
+    <row r="12" spans="1:70" s="47" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="47">
         <v>11</v>
       </c>
@@ -4392,7 +4393,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:70" s="51" customFormat="1" ht="28.9">
+    <row r="13" spans="1:70" s="51" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="59">
         <v>12</v>
       </c>
@@ -4426,7 +4427,7 @@
       <c r="K13" s="47"/>
       <c r="L13" s="47"/>
     </row>
-    <row r="14" spans="1:70" s="55" customFormat="1" ht="30.75">
+    <row r="14" spans="1:70" s="55" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="55">
         <v>13</v>
       </c>
@@ -4462,7 +4463,7 @@
       </c>
       <c r="L14" s="59"/>
     </row>
-    <row r="15" spans="1:70" s="21" customFormat="1" ht="30.75">
+    <row r="15" spans="1:70" s="21" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="21">
         <v>14</v>
       </c>
@@ -4497,7 +4498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:70" ht="28.9">
+    <row r="16" spans="1:70" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="79">
         <v>15</v>
       </c>
@@ -4589,7 +4590,7 @@
       <c r="BQ16" s="60"/>
       <c r="BR16" s="60"/>
     </row>
-    <row r="17" spans="1:12" s="10" customFormat="1" ht="76.5">
+    <row r="17" spans="1:12" s="10" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -4627,7 +4628,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="76.5">
+    <row r="18" spans="1:12" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -4665,7 +4666,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="21" customFormat="1" ht="28.9">
+    <row r="19" spans="1:12" s="21" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="84">
         <v>18</v>
       </c>
@@ -4697,7 +4698,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="76.5">
+    <row r="20" spans="1:12" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -4735,7 +4736,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="28.9">
+    <row r="21" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -4768,7 +4769,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="28.9">
+    <row r="22" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
         <v>21</v>
       </c>
@@ -4794,7 +4795,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="28.9">
+    <row r="23" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -4820,7 +4821,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="28.9">
+    <row r="24" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -4852,7 +4853,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="28.9">
+    <row r="25" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -4884,7 +4885,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="30.75">
+    <row r="26" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="23" t="s">
         <v>48</v>
@@ -4913,7 +4914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="28.9">
+    <row r="27" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="23" t="s">
         <v>48</v>
@@ -4939,7 +4940,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="28.9">
+    <row r="28" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>25</v>
       </c>
@@ -4971,7 +4972,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="106.5">
+    <row r="29" spans="1:12" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>26</v>
       </c>
@@ -5009,7 +5010,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="91.5">
+    <row r="30" spans="1:12" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>27</v>
       </c>
@@ -5047,7 +5048,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="76.5">
+    <row r="31" spans="1:12" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>28</v>
       </c>
@@ -5085,7 +5086,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="28.9">
+    <row r="32" spans="1:12" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
         <v>29</v>
       </c>
@@ -5109,7 +5110,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="106.5">
+    <row r="33" spans="1:12" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>30</v>
       </c>
@@ -5147,7 +5148,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="91.5">
+    <row r="34" spans="1:12" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>81</v>
       </c>
@@ -5181,7 +5182,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="30.75">
+    <row r="35" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>85</v>
       </c>
@@ -5210,7 +5211,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="30.75">
+    <row r="36" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>88</v>
       </c>
@@ -5246,7 +5247,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:12" s="8" customFormat="1" ht="30.75">
+    <row r="37" spans="1:12" s="8" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>32</v>
       </c>
@@ -5282,7 +5283,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:12" s="21" customFormat="1" ht="28.9">
+    <row r="38" spans="1:12" s="21" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="21">
         <v>33</v>
       </c>
@@ -5314,7 +5315,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:12" s="21" customFormat="1" ht="28.9">
+    <row r="39" spans="1:12" s="21" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="81">
         <v>34</v>
       </c>
@@ -5346,7 +5347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:12" s="10" customFormat="1" ht="28.9">
+    <row r="40" spans="1:12" s="10" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>35</v>
       </c>
@@ -5369,7 +5370,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="30.75">
+    <row r="41" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>36</v>
       </c>
@@ -5405,7 +5406,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="76.5">
+    <row r="42" spans="1:12" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>37</v>
       </c>
@@ -5443,7 +5444,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="76.5">
+    <row r="43" spans="1:12" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>38</v>
       </c>
@@ -5481,7 +5482,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="30.75">
+    <row r="44" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>39</v>
       </c>
@@ -5517,7 +5518,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="30.75">
+    <row r="45" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>40</v>
       </c>
@@ -5553,7 +5554,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="28.9">
+    <row r="46" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="10">
         <v>41</v>
       </c>
@@ -5579,7 +5580,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="28.9">
+    <row r="47" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>42</v>
       </c>
@@ -5605,7 +5606,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="28.9">
+    <row r="48" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>43</v>
       </c>
@@ -5631,7 +5632,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="49" spans="1:31" ht="28.9">
+    <row r="49" spans="1:31" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="39">
         <v>44</v>
       </c>
@@ -5655,7 +5656,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="50" spans="1:31" ht="28.9">
+    <row r="50" spans="1:31" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>45</v>
       </c>
@@ -5679,7 +5680,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="51" spans="1:31" ht="28.9">
+    <row r="51" spans="1:31" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>46</v>
       </c>
@@ -5695,15 +5696,20 @@
       <c r="E51" s="34">
         <v>4</v>
       </c>
-      <c r="F51" s="34"/>
+      <c r="F51" s="34" t="s">
+        <v>37</v>
+      </c>
       <c r="G51" s="34" t="s">
         <v>51</v>
       </c>
       <c r="H51" s="4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="52" spans="1:31" ht="28.9">
+      <c r="I51" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="52" spans="1:31" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>47</v>
       </c>
@@ -5727,7 +5733,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:31" ht="28.9">
+    <row r="53" spans="1:31" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>48</v>
       </c>
@@ -5751,7 +5757,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:31" ht="28.9">
+    <row r="54" spans="1:31" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>49</v>
       </c>
@@ -5775,7 +5781,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:31" ht="30.75">
+    <row r="55" spans="1:31" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>121</v>
       </c>
@@ -5813,7 +5819,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:31" ht="30.75">
+    <row r="56" spans="1:31" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>123</v>
       </c>
@@ -5851,7 +5857,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:31" ht="39" customHeight="1">
+    <row r="57" spans="1:31" ht="39" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>125</v>
       </c>
@@ -5882,7 +5888,7 @@
       <c r="K57" s="10"/>
       <c r="L57" s="10"/>
     </row>
-    <row r="58" spans="1:31" ht="30.75">
+    <row r="58" spans="1:31" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>128</v>
       </c>
@@ -5918,7 +5924,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="1:31" ht="36" customHeight="1">
+    <row r="59" spans="1:31" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>51</v>
       </c>
@@ -5954,7 +5960,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="60" spans="1:31" ht="37.5" customHeight="1">
+    <row r="60" spans="1:31" ht="37.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="23" t="s">
         <v>101</v>
       </c>
@@ -5986,7 +5992,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="61" spans="1:31" ht="60.75">
+    <row r="61" spans="1:31" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="B61" s="23" t="s">
         <v>101</v>
       </c>
@@ -6018,7 +6024,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="62" spans="1:31" ht="28.9">
+    <row r="62" spans="1:31" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="8">
         <v>52</v>
       </c>
@@ -6070,7 +6076,7 @@
       <c r="AC62" s="8"/>
       <c r="AD62" s="8"/>
     </row>
-    <row r="63" spans="1:31" s="8" customFormat="1" ht="30.75">
+    <row r="63" spans="1:31" s="8" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>53</v>
       </c>
@@ -6125,7 +6131,7 @@
       <c r="AD63" s="4"/>
       <c r="AE63" s="104"/>
     </row>
-    <row r="64" spans="1:31">
+    <row r="64" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A64" s="10"/>
       <c r="B64" s="46"/>
       <c r="C64" s="46"/>
@@ -6157,7 +6163,7 @@
       <c r="AC64" s="10"/>
       <c r="AD64" s="10"/>
     </row>
-    <row r="65" spans="1:31">
+    <row r="65" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B65" s="27"/>
       <c r="C65" s="27"/>
       <c r="D65" s="43"/>
@@ -6165,7 +6171,7 @@
       <c r="F65" s="11"/>
       <c r="G65" s="11"/>
     </row>
-    <row r="66" spans="1:31">
+    <row r="66" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B66" s="27"/>
       <c r="C66" s="31"/>
       <c r="D66" s="43"/>
@@ -6173,7 +6179,7 @@
       <c r="F66" s="11"/>
       <c r="G66" s="11"/>
     </row>
-    <row r="67" spans="1:31">
+    <row r="67" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B67" s="27"/>
       <c r="C67" s="31"/>
       <c r="D67" s="43"/>
@@ -6181,7 +6187,7 @@
       <c r="F67" s="11"/>
       <c r="G67" s="11"/>
     </row>
-    <row r="68" spans="1:31" s="21" customFormat="1" ht="28.9">
+    <row r="68" spans="1:31" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="21">
         <v>54</v>
       </c>
@@ -6233,7 +6239,7 @@
       <c r="AC68" s="81"/>
       <c r="AD68" s="81"/>
     </row>
-    <row r="69" spans="1:31" s="9" customFormat="1" ht="30.75">
+    <row r="69" spans="1:31" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="9">
         <v>55</v>
       </c>
@@ -6288,7 +6294,7 @@
       <c r="AD69" s="4"/>
       <c r="AE69" s="105"/>
     </row>
-    <row r="70" spans="1:31" s="21" customFormat="1" ht="28.9">
+    <row r="70" spans="1:31" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="81">
         <v>56</v>
       </c>
@@ -6340,7 +6346,7 @@
       <c r="AC70" s="88"/>
       <c r="AD70" s="88"/>
     </row>
-    <row r="71" spans="1:31" s="9" customFormat="1" ht="28.9">
+    <row r="71" spans="1:31" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
         <v>56</v>
       </c>
@@ -6364,7 +6370,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="72" spans="1:31" s="21" customFormat="1" ht="28.9">
+    <row r="72" spans="1:31" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="88">
         <v>58</v>
       </c>
@@ -6396,7 +6402,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="73" spans="1:31" s="21" customFormat="1" ht="28.9">
+    <row r="73" spans="1:31" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="21">
         <v>59</v>
       </c>
@@ -6428,7 +6434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:31" s="21" customFormat="1" ht="28.9">
+    <row r="74" spans="1:31" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="81">
         <v>60</v>
       </c>
@@ -6460,7 +6466,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:31" s="10" customFormat="1" ht="28.9">
+    <row r="75" spans="1:31" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
         <v>61</v>
       </c>
@@ -6483,70 +6489,74 @@
         <v>92</v>
       </c>
     </row>
-    <row r="76" spans="1:31">
+    <row r="76" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A76" s="10"/>
       <c r="B76" s="26"/>
       <c r="C76" s="26"/>
       <c r="D76" s="26"/>
       <c r="G76" s="23"/>
     </row>
-    <row r="77" spans="1:31">
+    <row r="77" spans="1:31" x14ac:dyDescent="0.25">
       <c r="D77" s="23"/>
       <c r="G77" s="23"/>
     </row>
-    <row r="78" spans="1:31">
+    <row r="78" spans="1:31" x14ac:dyDescent="0.25">
       <c r="D78" s="23"/>
       <c r="G78" s="23"/>
     </row>
-    <row r="79" spans="1:31">
+    <row r="79" spans="1:31" x14ac:dyDescent="0.25">
       <c r="D79" s="23"/>
       <c r="G79" s="23"/>
     </row>
-    <row r="80" spans="1:31">
+    <row r="80" spans="1:31" x14ac:dyDescent="0.25">
       <c r="G80" s="23"/>
     </row>
-    <row r="81" spans="2:7">
+    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D81" s="23"/>
       <c r="G81" s="23"/>
     </row>
-    <row r="82" spans="2:7">
+    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D82" s="23"/>
       <c r="G82" s="23"/>
     </row>
-    <row r="83" spans="2:7" s="8" customFormat="1">
+    <row r="83" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B83" s="24"/>
       <c r="C83" s="24"/>
       <c r="D83" s="24"/>
       <c r="G83" s="24"/>
     </row>
-    <row r="84" spans="2:7">
+    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B84" s="27"/>
       <c r="C84" s="27"/>
       <c r="D84" s="43"/>
       <c r="E84" s="11"/>
     </row>
-    <row r="85" spans="2:7">
+    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B85" s="27"/>
       <c r="C85" s="27"/>
       <c r="D85" s="43"/>
       <c r="E85" s="11"/>
     </row>
-    <row r="86" spans="2:7">
+    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B86" s="27"/>
       <c r="C86" s="31"/>
       <c r="D86" s="43"/>
       <c r="E86" s="11"/>
     </row>
-    <row r="87" spans="2:7">
+    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B87" s="27"/>
       <c r="C87" s="31"/>
       <c r="D87" s="43"/>
       <c r="E87" s="11"/>
     </row>
-    <row r="88" spans="2:7" ht="15"/>
-    <row r="89" spans="2:7" ht="15"/>
   </sheetData>
-  <autoFilter ref="A1:BR1" xr:uid="{FF50C64C-9D5B-44C0-8C71-AEDF26F82C35}"/>
+  <autoFilter ref="A1:BR63" xr:uid="{FF50C64C-9D5B-44C0-8C71-AEDF26F82C35}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="1"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6557,7 +6567,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="45.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
@@ -6565,18 +6575,18 @@
     <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6">
-      <c r="B2" s="114" t="s">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="106" t="s">
         <v>154</v>
       </c>
-      <c r="C2" s="106" t="s">
+      <c r="C2" s="108" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="106"/>
-      <c r="E2" s="107"/>
-    </row>
-    <row r="3" spans="2:6">
-      <c r="B3" s="115"/>
+      <c r="D2" s="108"/>
+      <c r="E2" s="109"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="107"/>
       <c r="C3" s="19" t="s">
         <v>13</v>
       </c>
@@ -6590,7 +6600,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:6">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
         <v>156</v>
       </c>
@@ -6607,7 +6617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="13" t="s">
         <v>158</v>
       </c>
@@ -6624,7 +6634,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="13" t="s">
         <v>159</v>
       </c>
@@ -6641,7 +6651,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:6">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="13" t="s">
         <v>160</v>
       </c>
@@ -6658,7 +6668,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:6">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="13" t="s">
         <v>161</v>
       </c>
@@ -6675,7 +6685,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:6">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
         <v>162</v>
       </c>
@@ -6692,7 +6702,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:6">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="13" t="s">
         <v>163</v>
       </c>
@@ -6709,7 +6719,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:6">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="13" t="s">
         <v>164</v>
       </c>
@@ -6726,7 +6736,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="2:6">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="13" t="s">
         <v>165</v>
       </c>
@@ -6743,7 +6753,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="2:6">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="13" t="s">
         <v>166</v>
       </c>
@@ -6760,7 +6770,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="2:6">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="13" t="s">
         <v>167</v>
       </c>
@@ -6777,7 +6787,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:6">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="13" t="s">
         <v>168</v>
       </c>
@@ -6794,7 +6804,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:6">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="13" t="s">
         <v>169</v>
       </c>
@@ -6811,7 +6821,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="2:6">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="13" t="s">
         <v>171</v>
       </c>
@@ -6828,7 +6838,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="2:6">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="13" t="s">
         <v>172</v>
       </c>
@@ -6845,7 +6855,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="2:6">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="13" t="s">
         <v>173</v>
       </c>
@@ -6862,7 +6872,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="2:6">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="13" t="s">
         <v>174</v>
       </c>
@@ -6877,7 +6887,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="2:6">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="13" t="s">
         <v>175</v>
       </c>
@@ -6890,7 +6900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:6">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="13" t="s">
         <v>176</v>
       </c>
@@ -6905,7 +6915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:6">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="13" t="s">
         <v>177</v>
       </c>
@@ -6920,7 +6930,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="2:6">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="13" t="s">
         <v>178</v>
       </c>
@@ -6935,7 +6945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:6">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="13" t="s">
         <v>179</v>
       </c>
@@ -6952,7 +6962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:6">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="13" t="s">
         <v>180</v>
       </c>
@@ -6969,7 +6979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:6">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="13" t="s">
         <v>181</v>
       </c>
@@ -6986,7 +6996,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="2:6">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="13" t="s">
         <v>182</v>
       </c>
@@ -7003,7 +7013,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="2:6">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="13" t="s">
         <v>183</v>
       </c>
@@ -7020,7 +7030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:6">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="13" t="s">
         <v>184</v>
       </c>
@@ -7037,7 +7047,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="2:6">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="16" t="s">
         <v>185</v>
       </c>
@@ -7069,7 +7079,7 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.42578125" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
@@ -7086,12 +7096,12 @@
     <col min="13" max="13" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L3" s="65" t="s">
         <v>187</v>
       </c>
@@ -7099,7 +7109,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="61" t="s">
         <v>189</v>
       </c>
@@ -7132,7 +7142,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="63" t="s">
         <v>3</v>
       </c>
@@ -7167,7 +7177,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>188</v>
       </c>
@@ -7181,7 +7191,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L7" s="27" t="s">
         <v>198</v>
       </c>
@@ -7189,7 +7199,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L8" s="27" t="s">
         <v>199</v>
       </c>
@@ -7197,7 +7207,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="66" t="s">
         <v>200</v>
       </c>
@@ -7211,7 +7221,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="68" t="s">
         <v>203</v>
       </c>
@@ -7223,7 +7233,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="70" t="s">
         <v>205</v>
       </c>
@@ -7237,7 +7247,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L12" s="27" t="s">
         <v>208</v>
       </c>
@@ -7245,7 +7255,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L13" s="27" t="s">
         <v>209</v>
       </c>
@@ -7253,7 +7263,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L14" s="27" t="s">
         <v>210</v>
       </c>
@@ -7261,7 +7271,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L15" s="27" t="s">
         <v>211</v>
       </c>
@@ -7269,7 +7279,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L16" s="27" t="s">
         <v>212</v>
       </c>
@@ -7277,12 +7287,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="61" t="s">
         <v>189</v>
       </c>
@@ -7309,7 +7319,7 @@
       </c>
       <c r="I20" s="73"/>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="63" t="s">
         <v>3</v>
       </c>
@@ -7338,7 +7348,7 @@
       </c>
       <c r="I21" s="74"/>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>188</v>
       </c>
@@ -7346,7 +7356,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="J23" s="93" t="s">
         <v>1</v>
       </c>
@@ -7360,11 +7370,11 @@
         <v>188</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="15" customHeight="1">
-      <c r="J24" s="109" t="s">
+    <row r="24" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J24" s="115" t="s">
         <v>215</v>
       </c>
-      <c r="K24" s="108" t="s">
+      <c r="K24" s="112" t="s">
         <v>216</v>
       </c>
       <c r="L24" s="72" t="s">
@@ -7374,15 +7384,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="42" customHeight="1">
+    <row r="25" spans="1:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="96" t="s">
         <v>200</v>
       </c>
       <c r="B25" s="97">
         <v>7</v>
       </c>
-      <c r="J25" s="109"/>
-      <c r="K25" s="108"/>
+      <c r="J25" s="115"/>
+      <c r="K25" s="112"/>
       <c r="L25" s="72" t="s">
         <v>218</v>
       </c>
@@ -7390,14 +7400,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="45" customHeight="1">
+    <row r="26" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="98" t="s">
         <v>205</v>
       </c>
       <c r="B26" s="99">
         <v>5</v>
       </c>
-      <c r="J26" s="109"/>
+      <c r="J26" s="115"/>
       <c r="K26" s="92" t="s">
         <v>219</v>
       </c>
@@ -7408,12 +7418,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="38.25" customHeight="1">
-      <c r="A27" s="112" t="s">
+    <row r="27" spans="1:13" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="110" t="s">
         <v>221</v>
       </c>
-      <c r="B27" s="113"/>
-      <c r="J27" s="109"/>
+      <c r="B27" s="111"/>
+      <c r="J27" s="115"/>
       <c r="K27" s="16" t="s">
         <v>222</v>
       </c>
@@ -7424,9 +7434,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
-      <c r="J28" s="109"/>
-      <c r="K28" s="108" t="s">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J28" s="115"/>
+      <c r="K28" s="112" t="s">
         <v>224</v>
       </c>
       <c r="L28" s="72" t="s">
@@ -7436,9 +7446,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
-      <c r="J29" s="109"/>
-      <c r="K29" s="108"/>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J29" s="115"/>
+      <c r="K29" s="112"/>
       <c r="L29" s="72" t="s">
         <v>226</v>
       </c>
@@ -7446,9 +7456,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
-      <c r="J30" s="109"/>
-      <c r="K30" s="108"/>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J30" s="115"/>
+      <c r="K30" s="112"/>
       <c r="L30" s="72" t="s">
         <v>227</v>
       </c>
@@ -7456,9 +7466,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
-      <c r="J31" s="109"/>
-      <c r="K31" s="108"/>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J31" s="115"/>
+      <c r="K31" s="112"/>
       <c r="L31" s="72" t="s">
         <v>228</v>
       </c>
@@ -7466,8 +7476,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="28.9">
-      <c r="J32" s="110" t="s">
+    <row r="32" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="J32" s="113" t="s">
         <v>229</v>
       </c>
       <c r="K32" s="94" t="s">
@@ -7480,9 +7490,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="10:13">
-      <c r="J33" s="108"/>
-      <c r="K33" s="108" t="s">
+    <row r="33" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J33" s="112"/>
+      <c r="K33" s="112" t="s">
         <v>216</v>
       </c>
       <c r="L33" s="27" t="s">
@@ -7492,9 +7502,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="10:13">
-      <c r="J34" s="108"/>
-      <c r="K34" s="108"/>
+    <row r="34" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J34" s="112"/>
+      <c r="K34" s="112"/>
       <c r="L34" s="27" t="s">
         <v>231</v>
       </c>
@@ -7502,9 +7512,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="10:13">
-      <c r="J35" s="108"/>
-      <c r="K35" s="108"/>
+    <row r="35" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J35" s="112"/>
+      <c r="K35" s="112"/>
       <c r="L35" s="27" t="s">
         <v>232</v>
       </c>
@@ -7512,9 +7522,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="10:13">
-      <c r="J36" s="108"/>
-      <c r="K36" s="108" t="s">
+    <row r="36" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J36" s="112"/>
+      <c r="K36" s="112" t="s">
         <v>184</v>
       </c>
       <c r="L36" s="27" t="s">
@@ -7524,9 +7534,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="10:13">
-      <c r="J37" s="108"/>
-      <c r="K37" s="108"/>
+    <row r="37" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J37" s="112"/>
+      <c r="K37" s="112"/>
       <c r="L37" s="27" t="s">
         <v>234</v>
       </c>
@@ -7534,9 +7544,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="10:13">
-      <c r="J38" s="108"/>
-      <c r="K38" s="108"/>
+    <row r="38" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J38" s="112"/>
+      <c r="K38" s="112"/>
       <c r="L38" s="27" t="s">
         <v>235</v>
       </c>
@@ -7544,9 +7554,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="10:13">
-      <c r="J39" s="108"/>
-      <c r="K39" s="108"/>
+    <row r="39" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J39" s="112"/>
+      <c r="K39" s="112"/>
       <c r="L39" s="27" t="s">
         <v>236</v>
       </c>
@@ -7554,9 +7564,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="10:13">
-      <c r="J40" s="111"/>
-      <c r="K40" s="111"/>
+    <row r="40" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J40" s="114"/>
+      <c r="K40" s="114"/>
       <c r="L40" s="45" t="s">
         <v>237</v>
       </c>
@@ -7564,11 +7574,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="10:13">
-      <c r="J41" s="108" t="s">
+    <row r="41" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J41" s="112" t="s">
         <v>238</v>
       </c>
-      <c r="K41" s="108" t="s">
+      <c r="K41" s="112" t="s">
         <v>239</v>
       </c>
       <c r="L41" s="27" t="s">
@@ -7578,9 +7588,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="10:13">
-      <c r="J42" s="108"/>
-      <c r="K42" s="108"/>
+    <row r="42" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J42" s="112"/>
+      <c r="K42" s="112"/>
       <c r="L42" s="27" t="s">
         <v>241</v>
       </c>
@@ -7588,9 +7598,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="10:13">
-      <c r="J43" s="108"/>
-      <c r="K43" s="108"/>
+    <row r="43" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J43" s="112"/>
+      <c r="K43" s="112"/>
       <c r="L43" s="27" t="s">
         <v>242</v>
       </c>
@@ -7598,9 +7608,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="10:13">
-      <c r="J44" s="108"/>
-      <c r="K44" s="108"/>
+    <row r="44" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J44" s="112"/>
+      <c r="K44" s="112"/>
       <c r="L44" s="27" t="s">
         <v>243</v>
       </c>
@@ -7608,9 +7618,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="10:13">
-      <c r="J45" s="108"/>
-      <c r="K45" s="108"/>
+    <row r="45" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J45" s="112"/>
+      <c r="K45" s="112"/>
       <c r="L45" s="27" t="s">
         <v>244</v>
       </c>
@@ -7618,9 +7628,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="10:13">
-      <c r="J46" s="108"/>
-      <c r="K46" s="108"/>
+    <row r="46" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J46" s="112"/>
+      <c r="K46" s="112"/>
       <c r="L46" s="27" t="s">
         <v>245</v>
       </c>
@@ -7628,9 +7638,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="10:13">
-      <c r="J47" s="108"/>
-      <c r="K47" s="108"/>
+    <row r="47" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J47" s="112"/>
+      <c r="K47" s="112"/>
       <c r="L47" s="27" t="s">
         <v>246</v>
       </c>
@@ -7638,8 +7648,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="10:13" ht="28.9">
-      <c r="J48" s="108"/>
+    <row r="48" spans="10:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="J48" s="112"/>
       <c r="K48" s="92" t="s">
         <v>247</v>
       </c>
@@ -7650,8 +7660,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:13">
-      <c r="J49" s="108"/>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J49" s="112"/>
       <c r="K49" s="16" t="s">
         <v>248</v>
       </c>
@@ -7662,8 +7672,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:13">
-      <c r="J50" s="108"/>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J50" s="112"/>
       <c r="K50" s="16" t="s">
         <v>219</v>
       </c>
@@ -7674,17 +7684,17 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M51">
         <v>187</v>
       </c>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="15">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="61" t="s">
         <v>189</v>
       </c>
@@ -7723,7 +7733,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="15">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="63" t="s">
         <v>3</v>
       </c>
@@ -7735,180 +7745,188 @@
       <c r="G57" s="17"/>
       <c r="H57" s="64"/>
       <c r="I57" s="74"/>
-      <c r="J57" s="109"/>
-      <c r="K57" s="108"/>
+      <c r="J57" s="115"/>
+      <c r="K57" s="112"/>
       <c r="L57" s="72"/>
       <c r="M57" s="72"/>
     </row>
-    <row r="58" spans="1:13" ht="15" customHeight="1">
+    <row r="58" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>188</v>
       </c>
-      <c r="J58" s="109"/>
-      <c r="K58" s="108"/>
+      <c r="J58" s="115"/>
+      <c r="K58" s="112"/>
       <c r="L58" s="72"/>
       <c r="M58" s="72"/>
     </row>
-    <row r="59" spans="1:13" ht="15" customHeight="1">
-      <c r="J59" s="109"/>
+    <row r="59" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J59" s="115"/>
       <c r="K59" s="92"/>
       <c r="L59" s="72"/>
       <c r="M59" s="72"/>
     </row>
-    <row r="60" spans="1:13" ht="15" customHeight="1">
-      <c r="J60" s="109"/>
+    <row r="60" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J60" s="115"/>
       <c r="K60" s="16"/>
       <c r="L60" s="72"/>
       <c r="M60" s="72"/>
     </row>
-    <row r="61" spans="1:13" ht="15" customHeight="1">
-      <c r="J61" s="109"/>
-      <c r="K61" s="108"/>
+    <row r="61" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J61" s="115"/>
+      <c r="K61" s="112"/>
       <c r="L61" s="72"/>
       <c r="M61" s="72"/>
     </row>
-    <row r="62" spans="1:13" ht="15" customHeight="1">
-      <c r="J62" s="109"/>
-      <c r="K62" s="108"/>
+    <row r="62" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J62" s="115"/>
+      <c r="K62" s="112"/>
       <c r="L62" s="72"/>
       <c r="M62" s="72"/>
     </row>
-    <row r="63" spans="1:13" ht="15" customHeight="1">
-      <c r="J63" s="109"/>
-      <c r="K63" s="108"/>
+    <row r="63" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J63" s="115"/>
+      <c r="K63" s="112"/>
       <c r="L63" s="72"/>
       <c r="M63" s="72"/>
     </row>
-    <row r="64" spans="1:13" ht="15" customHeight="1">
-      <c r="J64" s="109"/>
-      <c r="K64" s="108"/>
+    <row r="64" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J64" s="115"/>
+      <c r="K64" s="112"/>
       <c r="L64" s="72"/>
       <c r="M64" s="72"/>
     </row>
-    <row r="65" spans="10:13" ht="15" customHeight="1">
-      <c r="J65" s="110"/>
+    <row r="65" spans="10:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J65" s="113"/>
       <c r="K65" s="94"/>
       <c r="L65" s="95"/>
       <c r="M65" s="27"/>
     </row>
-    <row r="66" spans="10:13" ht="14.45" customHeight="1">
-      <c r="J66" s="108"/>
-      <c r="K66" s="108"/>
+    <row r="66" spans="10:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J66" s="112"/>
+      <c r="K66" s="112"/>
       <c r="L66" s="27"/>
       <c r="M66" s="27"/>
     </row>
-    <row r="67" spans="10:13" ht="14.45" customHeight="1">
-      <c r="J67" s="108"/>
-      <c r="K67" s="108"/>
+    <row r="67" spans="10:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J67" s="112"/>
+      <c r="K67" s="112"/>
       <c r="L67" s="27"/>
       <c r="M67" s="27"/>
     </row>
-    <row r="68" spans="10:13" ht="14.45" customHeight="1">
-      <c r="J68" s="108"/>
-      <c r="K68" s="108"/>
+    <row r="68" spans="10:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J68" s="112"/>
+      <c r="K68" s="112"/>
       <c r="L68" s="27"/>
       <c r="M68" s="27"/>
     </row>
-    <row r="69" spans="10:13" ht="14.45" customHeight="1">
-      <c r="J69" s="108"/>
-      <c r="K69" s="108"/>
+    <row r="69" spans="10:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J69" s="112"/>
+      <c r="K69" s="112"/>
       <c r="L69" s="27"/>
       <c r="M69" s="27"/>
     </row>
-    <row r="70" spans="10:13" ht="14.45" customHeight="1">
-      <c r="J70" s="108"/>
-      <c r="K70" s="108"/>
+    <row r="70" spans="10:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J70" s="112"/>
+      <c r="K70" s="112"/>
       <c r="L70" s="27"/>
       <c r="M70" s="27"/>
     </row>
-    <row r="71" spans="10:13" ht="14.45" customHeight="1">
-      <c r="J71" s="108"/>
-      <c r="K71" s="108"/>
+    <row r="71" spans="10:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J71" s="112"/>
+      <c r="K71" s="112"/>
       <c r="L71" s="27"/>
       <c r="M71" s="27"/>
     </row>
-    <row r="72" spans="10:13" ht="14.45" customHeight="1">
-      <c r="J72" s="108"/>
-      <c r="K72" s="108"/>
+    <row r="72" spans="10:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J72" s="112"/>
+      <c r="K72" s="112"/>
       <c r="L72" s="27"/>
       <c r="M72" s="27"/>
     </row>
-    <row r="73" spans="10:13" ht="14.45" customHeight="1">
-      <c r="J73" s="111"/>
-      <c r="K73" s="111"/>
+    <row r="73" spans="10:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J73" s="114"/>
+      <c r="K73" s="114"/>
       <c r="L73" s="45"/>
       <c r="M73" s="45"/>
     </row>
-    <row r="74" spans="10:13" ht="14.45" customHeight="1">
-      <c r="J74" s="108" t="s">
+    <row r="74" spans="10:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J74" s="112" t="s">
         <v>238</v>
       </c>
-      <c r="K74" s="108" t="s">
+      <c r="K74" s="112" t="s">
         <v>239</v>
       </c>
       <c r="L74" s="27"/>
       <c r="M74" s="27"/>
     </row>
-    <row r="75" spans="10:13" ht="14.45" customHeight="1">
-      <c r="J75" s="108"/>
-      <c r="K75" s="108"/>
+    <row r="75" spans="10:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J75" s="112"/>
+      <c r="K75" s="112"/>
       <c r="L75" s="27"/>
       <c r="M75" s="27"/>
     </row>
-    <row r="76" spans="10:13" ht="14.45" customHeight="1">
-      <c r="J76" s="108"/>
-      <c r="K76" s="108"/>
+    <row r="76" spans="10:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J76" s="112"/>
+      <c r="K76" s="112"/>
       <c r="L76" s="27"/>
       <c r="M76" s="27"/>
     </row>
-    <row r="77" spans="10:13" ht="14.45" customHeight="1">
-      <c r="J77" s="108"/>
-      <c r="K77" s="108"/>
+    <row r="77" spans="10:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J77" s="112"/>
+      <c r="K77" s="112"/>
       <c r="L77" s="27"/>
       <c r="M77" s="27"/>
     </row>
-    <row r="78" spans="10:13" ht="14.45" customHeight="1">
-      <c r="J78" s="108"/>
-      <c r="K78" s="108"/>
+    <row r="78" spans="10:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J78" s="112"/>
+      <c r="K78" s="112"/>
       <c r="L78" s="27"/>
       <c r="M78" s="27"/>
     </row>
-    <row r="79" spans="10:13" ht="14.45" customHeight="1">
-      <c r="J79" s="108"/>
-      <c r="K79" s="108"/>
+    <row r="79" spans="10:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J79" s="112"/>
+      <c r="K79" s="112"/>
       <c r="L79" s="27"/>
       <c r="M79" s="27"/>
     </row>
-    <row r="80" spans="10:13" ht="14.45" customHeight="1">
-      <c r="J80" s="108"/>
-      <c r="K80" s="108"/>
+    <row r="80" spans="10:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J80" s="112"/>
+      <c r="K80" s="112"/>
       <c r="L80" s="27"/>
       <c r="M80" s="27"/>
     </row>
-    <row r="81" spans="10:13" ht="15" customHeight="1">
-      <c r="J81" s="108"/>
+    <row r="81" spans="10:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J81" s="112"/>
       <c r="K81" s="92" t="s">
         <v>251</v>
       </c>
       <c r="L81" s="31"/>
       <c r="M81" s="27"/>
     </row>
-    <row r="82" spans="10:13" ht="14.45" customHeight="1">
-      <c r="J82" s="108"/>
+    <row r="82" spans="10:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J82" s="112"/>
       <c r="K82" s="16" t="s">
         <v>252</v>
       </c>
       <c r="L82" s="27"/>
       <c r="M82" s="27"/>
     </row>
-    <row r="83" spans="10:13" ht="15" customHeight="1">
-      <c r="J83" s="108"/>
+    <row r="83" spans="10:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J83" s="112"/>
       <c r="K83" s="16"/>
       <c r="L83" s="91"/>
       <c r="M83" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="J74:J83"/>
+    <mergeCell ref="K74:K80"/>
+    <mergeCell ref="J57:J64"/>
+    <mergeCell ref="K57:K58"/>
+    <mergeCell ref="K61:K64"/>
+    <mergeCell ref="J65:J73"/>
+    <mergeCell ref="K66:K68"/>
+    <mergeCell ref="K69:K73"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="K41:K47"/>
     <mergeCell ref="J41:J50"/>
@@ -7918,14 +7936,6 @@
     <mergeCell ref="K24:K25"/>
     <mergeCell ref="K36:K40"/>
     <mergeCell ref="K33:K35"/>
-    <mergeCell ref="J74:J83"/>
-    <mergeCell ref="K74:K80"/>
-    <mergeCell ref="J57:J64"/>
-    <mergeCell ref="K57:K58"/>
-    <mergeCell ref="K61:K64"/>
-    <mergeCell ref="J65:J73"/>
-    <mergeCell ref="K66:K68"/>
-    <mergeCell ref="K69:K73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7939,7 +7949,7 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.7109375" style="1"/>
     <col min="2" max="2" width="74" style="1" customWidth="1"/>
@@ -7947,22 +7957,22 @@
     <col min="4" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="28.9">
+    <row r="2" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="28.9">
+    <row r="3" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="28.9">
+    <row r="4" spans="2:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="43.9" customHeight="1">
+    <row r="5" spans="2:3" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>256</v>
       </c>
@@ -7970,92 +7980,92 @@
         <v>257</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="28.9">
+    <row r="6" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="28.9">
+    <row r="7" spans="2:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="43.15">
+    <row r="8" spans="2:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="28.9">
+    <row r="9" spans="2:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="43.15">
+    <row r="10" spans="2:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="28.9">
+    <row r="11" spans="2:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="28.9">
+    <row r="12" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="28.9">
+    <row r="13" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="28.9">
+    <row r="14" spans="2:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="15" spans="2:3" ht="28.9">
+    <row r="15" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="16" spans="2:3" ht="43.15">
+    <row r="16" spans="2:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="43.15">
+    <row r="17" spans="2:2" ht="45" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="28.9">
+    <row r="18" spans="2:2" ht="45" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="28.9">
+    <row r="19" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="43.15">
+    <row r="20" spans="2:2" ht="45" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="28.9">
+    <row r="21" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="22" spans="2:2" ht="28.9">
+    <row r="22" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="23" spans="2:2" ht="28.9">
+    <row r="23" spans="2:2" ht="45" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>275</v>
       </c>
@@ -8073,7 +8083,7 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
@@ -8090,7 +8100,7 @@
     <col min="15" max="15" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18">
+    <row r="1" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="28" t="s">
         <v>276</v>
       </c>
@@ -8137,7 +8147,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="144">
+    <row r="2" spans="1:15" ht="165" x14ac:dyDescent="0.25">
       <c r="A2" s="27">
         <v>1</v>
       </c>
@@ -8174,7 +8184,7 @@
       <c r="N2" s="27"/>
       <c r="O2" s="27"/>
     </row>
-    <row r="3" spans="1:15" ht="86.45">
+    <row r="3" spans="1:15" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="27">
         <v>2</v>
       </c>
@@ -8215,7 +8225,7 @@
       <c r="N3" s="27"/>
       <c r="O3" s="27"/>
     </row>
-    <row r="4" spans="1:15" ht="57.6">
+    <row r="4" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="27">
         <v>3</v>
       </c>
@@ -8252,7 +8262,7 @@
       <c r="N4" s="27"/>
       <c r="O4" s="45"/>
     </row>
-    <row r="5" spans="1:15" ht="158.44999999999999">
+    <row r="5" spans="1:15" ht="165" x14ac:dyDescent="0.25">
       <c r="A5" s="27">
         <v>5</v>
       </c>
@@ -8291,7 +8301,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="187.15">
+    <row r="6" spans="1:15" ht="195" x14ac:dyDescent="0.25">
       <c r="A6" s="27">
         <v>6</v>
       </c>
@@ -8332,7 +8342,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="57.6">
+    <row r="7" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="27">
         <v>7</v>
       </c>
@@ -8371,7 +8381,7 @@
       </c>
       <c r="O7" s="27"/>
     </row>
-    <row r="8" spans="1:15" ht="57.6">
+    <row r="8" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="27">
         <v>8</v>
       </c>
@@ -8412,7 +8422,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="57.6">
+    <row r="9" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="27">
         <v>9</v>
       </c>
@@ -8449,7 +8459,7 @@
       <c r="N9" s="27"/>
       <c r="O9" s="27"/>
     </row>
-    <row r="10" spans="1:15" ht="57.6">
+    <row r="10" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="27">
         <v>10</v>
       </c>
@@ -8488,7 +8498,7 @@
       <c r="N10" s="27"/>
       <c r="O10" s="27"/>
     </row>
-    <row r="11" spans="1:15" ht="374.45">
+    <row r="11" spans="1:15" ht="390" x14ac:dyDescent="0.25">
       <c r="A11" s="27">
         <v>12</v>
       </c>
@@ -8527,7 +8537,7 @@
       <c r="N11" s="27"/>
       <c r="O11" s="27"/>
     </row>
-    <row r="12" spans="1:15" ht="57.6">
+    <row r="12" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="27">
         <v>13</v>
       </c>
@@ -8564,7 +8574,7 @@
       <c r="N12" s="27"/>
       <c r="O12" s="27"/>
     </row>
-    <row r="13" spans="1:15" ht="57.6">
+    <row r="13" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="27">
         <v>14</v>
       </c>
@@ -8603,7 +8613,7 @@
       <c r="N13" s="27"/>
       <c r="O13" s="27"/>
     </row>
-    <row r="14" spans="1:15" ht="237.75" customHeight="1">
+    <row r="14" spans="1:15" ht="237.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="27">
         <v>15</v>
       </c>
@@ -8640,7 +8650,7 @@
       <c r="N14" s="27"/>
       <c r="O14" s="27"/>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>16</v>
       </c>
@@ -8651,7 +8661,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>17</v>
       </c>
@@ -8662,7 +8672,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="17" spans="3:3" ht="100.9">
+    <row r="17" spans="3:3" ht="105" x14ac:dyDescent="0.25">
       <c r="C17" s="32" t="s">
         <v>327</v>
       </c>

</xml_diff>